<commit_message>
feat: texto padrão e tipo de projeto
</commit_message>
<xml_diff>
--- a/output_path.xlsx
+++ b/output_path.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,215 +440,64 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>SONDAGEM A TRADO</t>
+          <t>SONDAGEM MISTA</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>MEDIÇÃO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>NORTE</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>LESTE</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>PROFUNDIDADE EXECUTADA (m)</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>MEDIÇÃO</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>UMIDADE NATURAL</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>DENSIDADE IN SITU</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>LL-LP</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>ANÁLISE GRANULOMÉTRICA COM PENEIRAMENTO E SEDIMENTAÇÃO</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>COMPACTAÇÃO E CBR (5 PONTOS) ENERGIA PROCTOR NORMAL</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>COMPACTAÇÃO E CBR (5 PONTOS) ENERGIA PROCTOR INTERMEDIÁRIO</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>MCT-PASTILHAS</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>MÓDULO DE RESILIÊNCIA</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ST-km049-101</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>N=250300.1382</t>
-        </is>
+          <t>SM-km050-001</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>45658</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>E=151134.0721</t>
+          <t>N=250362.5494</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>45809</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1</v>
-      </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
+          <t>E=151188.7322</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ST-km049-102</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>N=250306.0219</t>
-        </is>
+          <t>SM-km050-002</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>45658</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>E=151287.1549</t>
+          <t>N=250248.7755</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>45809</v>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ST-km050-101</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>N=250309.5521</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>E=151429.6398</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>45809</v>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ST-km050-102</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>N=250314.2590</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>E=151621.5822</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="n">
-        <v>2</v>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
+          <t>E=151378.0133</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>